<commit_message>
finished cohort logic and updated sparse matrix
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2013_2014.xlsx
+++ b/CDSData/CDS_SPARSE_2013_2014.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959E8906-F894-42EB-A14C-0359DBB8FB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BC5212-8375-440F-A27A-F62CC68E8F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7704" yWindow="4320" windowWidth="15336" windowHeight="8040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013 Cohort" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Value</t>
   </si>
@@ -45,12 +45,6 @@
     <t>any-aid</t>
   </si>
   <si>
-    <t>exclusions</t>
-  </si>
-  <si>
-    <t>adjusted</t>
-  </si>
-  <si>
     <t>within-4-years</t>
   </si>
   <si>
@@ -64,6 +58,15 @@
   </si>
   <si>
     <t>graduation-rate</t>
+  </si>
+  <si>
+    <t>exemptions</t>
+  </si>
+  <si>
+    <t>initial</t>
+  </si>
+  <si>
+    <t>final</t>
   </si>
 </sst>
 </file>
@@ -381,15 +384,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,28 +416,31 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>84</v>
       </c>
@@ -470,8 +480,11 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>185</v>
       </c>
@@ -511,8 +524,11 @@
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>290</v>
       </c>
@@ -552,8 +568,11 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>559</v>
       </c>
@@ -593,8 +612,11 @@
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -634,8 +656,11 @@
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -675,8 +700,11 @@
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -716,8 +744,11 @@
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -757,8 +788,11 @@
       <c r="M9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>84</v>
       </c>
@@ -798,8 +832,11 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>184</v>
       </c>
@@ -839,8 +876,11 @@
       <c r="M11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>290</v>
       </c>
@@ -880,8 +920,11 @@
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>558</v>
       </c>
@@ -921,8 +964,11 @@
       <c r="M13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>63</v>
       </c>
@@ -962,8 +1008,11 @@
       <c r="M14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>151</v>
       </c>
@@ -1003,8 +1052,11 @@
       <c r="M15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>216</v>
       </c>
@@ -1044,8 +1096,11 @@
       <c r="M16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>430</v>
       </c>
@@ -1085,8 +1140,11 @@
       <c r="M17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -1126,8 +1184,11 @@
       <c r="M18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>11</v>
       </c>
@@ -1167,8 +1228,11 @@
       <c r="M19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1208,8 +1272,11 @@
       <c r="M20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>38</v>
       </c>
@@ -1249,8 +1316,11 @@
       <c r="M21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1290,8 +1360,11 @@
       <c r="M22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1331,8 +1404,11 @@
       <c r="M23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1372,8 +1448,11 @@
       <c r="M24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1413,8 +1492,11 @@
       <c r="M25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>71</v>
       </c>
@@ -1454,8 +1536,11 @@
       <c r="M26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>165</v>
       </c>
@@ -1495,8 +1580,11 @@
       <c r="M27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>238</v>
       </c>
@@ -1536,8 +1624,11 @@
       <c r="M28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>474</v>
       </c>
@@ -1577,8 +1668,11 @@
       <c r="M29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>84.5</v>
       </c>
@@ -1618,8 +1712,11 @@
       <c r="M30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>89.7</v>
       </c>
@@ -1659,8 +1756,11 @@
       <c r="M31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>82.1</v>
       </c>
@@ -1700,8 +1800,11 @@
       <c r="M32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>84.9</v>
       </c>
@@ -1740,6 +1843,9 @@
       </c>
       <c r="M33">
         <v>1</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed test cases failing
</commit_message>
<xml_diff>
--- a/CDSData/CDS_SPARSE_2013_2014.xlsx
+++ b/CDSData/CDS_SPARSE_2013_2014.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BC5212-8375-440F-A27A-F62CC68E8F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFE3EC4-E900-4BA5-9432-3DF86EC475FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7704" yWindow="4320" windowWidth="15336" windowHeight="8040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2013 Cohort" sheetId="1" r:id="rId1"/>
+    <sheet name="2013_Cohort" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -387,7 +387,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>